<commit_message>
add test + bcubed metrics
</commit_message>
<xml_diff>
--- a/regression/ormodels.xlsx
+++ b/regression/ormodels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Диплом\Classerizption-of-banks\regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4E2910-E5F7-4CF3-952C-8CDDAB17959B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB554710-D076-49F3-80CB-B14B6A5E76AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="orprobit" sheetId="2" r:id="rId1"/>
@@ -960,9 +960,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -1334,7 +1333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{019CCCF3-611D-4AFE-8360-9509FCB322C6}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -1365,583 +1364,583 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="3"/>
+      <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>77</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>79</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>84</v>
       </c>
-      <c r="F17" s="3"/>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>87</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>89</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>93</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>94</v>
       </c>
-      <c r="F19" s="3"/>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>99</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>101</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>102</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>104</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>108</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>109</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>110</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>112</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>113</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>114</v>
       </c>
-      <c r="F23" s="3"/>
+      <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>116</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>117</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>118</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>119</v>
       </c>
-      <c r="F24" s="2"/>
+      <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>120</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>121</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>122</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>123</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>124</v>
       </c>
-      <c r="F25" s="3"/>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>125</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>126</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>127</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>128</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>129</v>
       </c>
-      <c r="F26" s="2"/>
+      <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>130</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>131</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>132</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>133</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>134</v>
       </c>
-      <c r="F27" s="3"/>
+      <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>135</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>136</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>137</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>138</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>139</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>140</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>141</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>142</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>143</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>144</v>
       </c>
-      <c r="F29" s="3"/>
+      <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>145</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>146</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>147</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" t="s">
         <v>148</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>149</v>
       </c>
-      <c r="F30" s="2"/>
+      <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>150</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>151</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>152</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>153</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>154</v>
       </c>
-      <c r="F31" s="3"/>
+      <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>155</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>156</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>157</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" t="s">
         <v>158</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>159</v>
       </c>
-      <c r="F32" s="2"/>
+      <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>160</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>161</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>162</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" t="s">
         <v>163</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>164</v>
       </c>
-      <c r="F33" s="3"/>
+      <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F34" s="2"/>
+      <c r="F34" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1955,7 +1954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31154155-B3AD-4CD2-AAC2-7E7EA63E7C75}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -1984,546 +1983,546 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>165</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>166</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>167</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>169</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>170</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>171</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>173</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>174</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>175</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>178</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>179</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>181</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>182</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>183</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>185</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>186</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>187</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>189</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>190</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>191</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>193</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>194</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>195</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>197</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>198</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>199</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>201</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>202</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>203</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>204</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>205</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>206</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>208</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>209</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>211</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>212</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>213</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>215</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>216</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>217</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>219</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>220</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>221</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>223</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>224</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>225</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>227</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>228</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>229</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>231</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>232</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>233</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>235</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>236</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>237</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>239</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>240</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>241</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>110</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>243</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>244</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>245</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>247</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>248</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>249</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>120</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>251</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>252</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>253</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>125</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>255</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>256</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>257</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>130</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>259</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>260</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>261</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>135</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>263</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>264</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>265</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>140</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>267</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>268</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>269</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>145</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>271</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>272</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" t="s">
         <v>273</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>150</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>275</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>276</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>277</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>155</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>279</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>280</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" t="s">
         <v>281</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>160</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>283</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>284</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" t="s">
         <v>285</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>286</v>
       </c>
     </row>

</xml_diff>